<commit_message>
first multiple deals site scrapped
</commit_message>
<xml_diff>
--- a/oiadsites.xlsx
+++ b/oiadsites.xlsx
@@ -3921,21 +3921,17 @@
   </sheetPr>
   <dimension ref="A1:I444"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A406" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A443" activeCellId="0" pane="topLeft" sqref="A443"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A4" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="C26" activeCellId="0" pane="topLeft" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.9098039215686"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="98.0196078431372"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="49.9098039215686"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.9686274509804"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.9098039215686"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.5607843137255"/>
-    <col collapsed="false" hidden="false" max="257" min="8" style="0" width="49.9098039215686"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="83.0313725490196"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.0352941176471"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.6156862745098"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1" s="1">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="1" s="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3961,7 +3957,7 @@
         <v>7</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
         <v>8</v>
       </c>
@@ -3981,7 +3977,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
         <v>13</v>
       </c>
@@ -4001,7 +3997,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
         <v>17</v>
       </c>
@@ -4024,7 +4020,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
         <v>21</v>
       </c>
@@ -4047,7 +4043,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
         <v>23</v>
       </c>
@@ -4070,7 +4066,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
         <v>26</v>
       </c>
@@ -4093,7 +4089,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
         <v>28</v>
       </c>
@@ -4116,7 +4112,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
         <v>31</v>
       </c>
@@ -4139,7 +4135,7 @@
         <v>33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
         <v>34</v>
       </c>
@@ -4162,7 +4158,7 @@
         <v>33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="11">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
         <v>37</v>
       </c>
@@ -4182,7 +4178,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="12">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.05" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
         <v>40</v>
       </c>
@@ -4205,7 +4201,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="13">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.05" outlineLevel="0" r="13">
       <c r="A13" s="0" t="s">
         <v>43</v>
       </c>
@@ -4228,7 +4224,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="14">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.05" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
         <v>46</v>
       </c>
@@ -4251,7 +4247,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="15">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.05" outlineLevel="0" r="15">
       <c r="A15" s="0" t="s">
         <v>49</v>
       </c>
@@ -4274,7 +4270,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="16">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.05" outlineLevel="0" r="16">
       <c r="A16" s="0" t="s">
         <v>52</v>
       </c>
@@ -4297,7 +4293,7 @@
         <v>55</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="17">
       <c r="A17" s="0" t="s">
         <v>56</v>
       </c>
@@ -4320,7 +4316,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="18">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="18">
       <c r="A18" s="0" t="s">
         <v>60</v>
       </c>
@@ -4343,7 +4339,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="19">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="19">
       <c r="A19" s="0" t="s">
         <v>63</v>
       </c>
@@ -4363,7 +4359,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="20">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="20">
       <c r="A20" s="0" t="s">
         <v>66</v>
       </c>
@@ -4383,7 +4379,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="21">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.05" outlineLevel="0" r="21">
       <c r="A21" s="0" t="s">
         <v>68</v>
       </c>
@@ -4406,7 +4402,7 @@
         <v>71</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="22">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="22">
       <c r="A22" s="0" t="s">
         <v>72</v>
       </c>
@@ -4429,7 +4425,7 @@
         <v>74</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="23">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="23">
       <c r="A23" s="0" t="s">
         <v>75</v>
       </c>
@@ -4449,7 +4445,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="24">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="24">
       <c r="A24" s="0" t="s">
         <v>77</v>
       </c>
@@ -4472,7 +4468,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="25">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="25">
       <c r="A25" s="0" t="s">
         <v>80</v>
       </c>
@@ -4495,7 +4491,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="26">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.05" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
         <v>83</v>
       </c>
@@ -4503,7 +4499,7 @@
         <v>84</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>25</v>
@@ -4518,7 +4514,7 @@
         <v>85</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="27">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.05" outlineLevel="0" r="27">
       <c r="A27" s="0" t="s">
         <v>86</v>
       </c>
@@ -4541,7 +4537,7 @@
         <v>19</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="28">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.05" outlineLevel="0" r="28">
       <c r="A28" s="0" t="s">
         <v>89</v>
       </c>
@@ -4564,7 +4560,7 @@
         <v>91</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="29">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="29">
       <c r="A29" s="0" t="s">
         <v>92</v>
       </c>
@@ -4584,7 +4580,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="30">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
         <v>94</v>
       </c>
@@ -4607,7 +4603,7 @@
         <v>96</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="31">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.05" outlineLevel="0" r="31">
       <c r="A31" s="0" t="s">
         <v>97</v>
       </c>
@@ -4630,7 +4626,7 @@
         <v>96</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="32">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.05" outlineLevel="0" r="32">
       <c r="A32" s="0" t="s">
         <v>99</v>
       </c>
@@ -4653,7 +4649,7 @@
         <v>96</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="33">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="33">
       <c r="A33" s="0" t="s">
         <v>102</v>
       </c>
@@ -4679,7 +4675,7 @@
         <v>105</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="34">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.05" outlineLevel="0" r="34">
       <c r="A34" s="0" t="s">
         <v>106</v>
       </c>
@@ -4699,7 +4695,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="35">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="35">
       <c r="A35" s="0" t="s">
         <v>109</v>
       </c>
@@ -4722,7 +4718,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="36">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="36">
       <c r="A36" s="0" t="s">
         <v>113</v>
       </c>
@@ -4742,7 +4738,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="37">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="37">
       <c r="A37" s="0" t="s">
         <v>115</v>
       </c>
@@ -4765,7 +4761,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="38">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="38">
       <c r="A38" s="0" t="s">
         <v>118</v>
       </c>
@@ -4785,7 +4781,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="39">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.05" outlineLevel="0" r="39">
       <c r="A39" s="0" t="s">
         <v>120</v>
       </c>
@@ -4805,7 +4801,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="40">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.05" outlineLevel="0" r="40">
       <c r="A40" s="0" t="s">
         <v>122</v>
       </c>
@@ -4831,7 +4827,7 @@
         <v>33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="41">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.05" outlineLevel="0" r="41">
       <c r="A41" s="0" t="s">
         <v>125</v>
       </c>
@@ -4851,7 +4847,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="42">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="42">
       <c r="A42" s="0" t="s">
         <v>128</v>
       </c>
@@ -4871,7 +4867,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="43">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="43">
       <c r="A43" s="0" t="s">
         <v>130</v>
       </c>
@@ -4894,7 +4890,7 @@
         <v>132</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="44">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="44">
       <c r="A44" s="0" t="s">
         <v>133</v>
       </c>
@@ -4914,7 +4910,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="45">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="45">
       <c r="A45" s="0" t="s">
         <v>135</v>
       </c>
@@ -4937,7 +4933,7 @@
         <v>137</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="46">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="46">
       <c r="A46" s="0" t="s">
         <v>138</v>
       </c>
@@ -4957,7 +4953,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="47">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="47">
       <c r="A47" s="0" t="s">
         <v>140</v>
       </c>
@@ -4980,7 +4976,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="48">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="48">
       <c r="A48" s="0" t="s">
         <v>143</v>
       </c>
@@ -5003,7 +4999,7 @@
         <v>145</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="49">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="49">
       <c r="A49" s="0" t="s">
         <v>146</v>
       </c>
@@ -5029,7 +5025,7 @@
         <v>149</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="50">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="50">
       <c r="A50" s="0" t="s">
         <v>150</v>
       </c>
@@ -5052,7 +5048,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="51">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="51">
       <c r="A51" s="0" t="s">
         <v>153</v>
       </c>
@@ -5075,7 +5071,7 @@
         <v>155</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="52">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="52">
       <c r="A52" s="0" t="s">
         <v>156</v>
       </c>
@@ -5098,7 +5094,7 @@
         <v>158</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="53">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="53">
       <c r="A53" s="0" t="s">
         <v>159</v>
       </c>
@@ -5118,7 +5114,7 @@
         <v>161</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="54">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="54">
       <c r="A54" s="0" t="s">
         <v>162</v>
       </c>
@@ -5138,7 +5134,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="55">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="55">
       <c r="A55" s="0" t="s">
         <v>164</v>
       </c>
@@ -5161,7 +5157,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="56">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="56">
       <c r="A56" s="0" t="s">
         <v>167</v>
       </c>
@@ -5184,7 +5180,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="57">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="57">
       <c r="A57" s="0" t="s">
         <v>169</v>
       </c>
@@ -5207,7 +5203,7 @@
         <v>171</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="58">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="58">
       <c r="A58" s="0" t="s">
         <v>172</v>
       </c>
@@ -5227,7 +5223,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="59">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="59">
       <c r="A59" s="0" t="s">
         <v>175</v>
       </c>
@@ -5250,7 +5246,7 @@
         <v>33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="60">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="60">
       <c r="A60" s="0" t="s">
         <v>178</v>
       </c>
@@ -5270,7 +5266,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="61">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="61">
       <c r="A61" s="0" t="s">
         <v>180</v>
       </c>
@@ -5293,7 +5289,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="62">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="62">
       <c r="A62" s="0" t="s">
         <v>183</v>
       </c>
@@ -5313,7 +5309,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="63">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="63">
       <c r="A63" s="0" t="s">
         <v>185</v>
       </c>
@@ -5333,7 +5329,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="64">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="64">
       <c r="A64" s="0" t="s">
         <v>187</v>
       </c>
@@ -5359,7 +5355,7 @@
         <v>191</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="65">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="65">
       <c r="A65" s="0" t="s">
         <v>192</v>
       </c>
@@ -5382,7 +5378,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="66">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="66">
       <c r="A66" s="0" t="s">
         <v>196</v>
       </c>
@@ -5405,7 +5401,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="67">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="67">
       <c r="A67" s="0" t="s">
         <v>199</v>
       </c>
@@ -5428,7 +5424,7 @@
         <v>201</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="68">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="68">
       <c r="A68" s="0" t="s">
         <v>202</v>
       </c>
@@ -5451,7 +5447,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="69">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="69">
       <c r="A69" s="0" t="s">
         <v>205</v>
       </c>
@@ -5477,7 +5473,7 @@
         <v>208</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="70">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="70">
       <c r="A70" s="0" t="s">
         <v>209</v>
       </c>
@@ -5497,7 +5493,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="71">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="71">
       <c r="A71" s="0" t="s">
         <v>211</v>
       </c>
@@ -5517,7 +5513,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="72">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="72">
       <c r="A72" s="0" t="s">
         <v>213</v>
       </c>
@@ -5543,7 +5539,7 @@
         <v>216</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="73">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="73">
       <c r="A73" s="0" t="s">
         <v>217</v>
       </c>
@@ -5566,7 +5562,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="74">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="74">
       <c r="A74" s="0" t="s">
         <v>220</v>
       </c>
@@ -5589,7 +5585,7 @@
         <v>222</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="75">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="75">
       <c r="A75" s="0" t="s">
         <v>223</v>
       </c>
@@ -5612,7 +5608,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="76">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="76">
       <c r="A76" s="0" t="s">
         <v>226</v>
       </c>
@@ -5635,7 +5631,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="77">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="77">
       <c r="A77" s="0" t="s">
         <v>229</v>
       </c>
@@ -5658,7 +5654,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="78">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="78">
       <c r="A78" s="0" t="s">
         <v>232</v>
       </c>
@@ -5681,7 +5677,7 @@
         <v>235</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="79">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="79">
       <c r="A79" s="0" t="s">
         <v>236</v>
       </c>
@@ -5701,7 +5697,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="80">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="80">
       <c r="A80" s="0" t="s">
         <v>239</v>
       </c>
@@ -5724,7 +5720,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="81">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="81">
       <c r="A81" s="0" t="s">
         <v>243</v>
       </c>
@@ -5750,7 +5746,7 @@
         <v>208</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="82">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="82">
       <c r="A82" s="0" t="s">
         <v>246</v>
       </c>
@@ -5770,7 +5766,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="83">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="83">
       <c r="A83" s="0" t="s">
         <v>248</v>
       </c>
@@ -5793,7 +5789,7 @@
         <v>19</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="84">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.05" outlineLevel="0" r="84">
       <c r="A84" s="0" t="s">
         <v>251</v>
       </c>
@@ -5816,7 +5812,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="85">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="85">
       <c r="A85" s="0" t="s">
         <v>254</v>
       </c>
@@ -5836,7 +5832,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="86">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="86">
       <c r="A86" s="0" t="s">
         <v>256</v>
       </c>
@@ -5859,7 +5855,7 @@
         <v>258</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="87">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="87">
       <c r="A87" s="0" t="s">
         <v>259</v>
       </c>
@@ -5882,7 +5878,7 @@
         <v>261</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="88">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="88">
       <c r="A88" s="0" t="s">
         <v>262</v>
       </c>
@@ -5905,7 +5901,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="89">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="89">
       <c r="A89" s="0" t="s">
         <v>265</v>
       </c>
@@ -5931,7 +5927,7 @@
         <v>268</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="90">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="90">
       <c r="A90" s="0" t="s">
         <v>269</v>
       </c>
@@ -5951,7 +5947,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="91">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="91">
       <c r="A91" s="0" t="s">
         <v>271</v>
       </c>
@@ -5971,7 +5967,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="92">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="92">
       <c r="A92" s="0" t="s">
         <v>273</v>
       </c>
@@ -5994,7 +5990,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="93">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="93">
       <c r="A93" s="0" t="s">
         <v>276</v>
       </c>
@@ -6014,7 +6010,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="94">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="94">
       <c r="A94" s="0" t="s">
         <v>278</v>
       </c>
@@ -6040,7 +6036,7 @@
         <v>281</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="95">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="95">
       <c r="A95" s="0" t="s">
         <v>282</v>
       </c>
@@ -6063,7 +6059,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="96">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="96">
       <c r="A96" s="0" t="s">
         <v>286</v>
       </c>
@@ -6086,7 +6082,7 @@
         <v>289</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="97">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="97">
       <c r="A97" s="0" t="s">
         <v>290</v>
       </c>
@@ -6109,7 +6105,7 @@
         <v>292</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="98">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="98">
       <c r="A98" s="0" t="s">
         <v>293</v>
       </c>
@@ -6132,7 +6128,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="99">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="99">
       <c r="A99" s="0" t="s">
         <v>296</v>
       </c>
@@ -6152,7 +6148,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="100">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="100">
       <c r="A100" s="0" t="s">
         <v>298</v>
       </c>
@@ -6172,7 +6168,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="101">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="101">
       <c r="A101" s="0" t="s">
         <v>300</v>
       </c>
@@ -6192,7 +6188,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="102">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="102">
       <c r="A102" s="0" t="s">
         <v>302</v>
       </c>
@@ -6212,7 +6208,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="103">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="103">
       <c r="A103" s="0" t="s">
         <v>304</v>
       </c>
@@ -6235,7 +6231,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="104">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="104">
       <c r="A104" s="0" t="s">
         <v>307</v>
       </c>
@@ -6258,7 +6254,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="105">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="105">
       <c r="A105" s="0" t="s">
         <v>310</v>
       </c>
@@ -6281,7 +6277,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="106">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="106">
       <c r="A106" s="0" t="s">
         <v>313</v>
       </c>
@@ -6304,7 +6300,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="107">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="107">
       <c r="A107" s="0" t="s">
         <v>316</v>
       </c>
@@ -6324,7 +6320,7 @@
         <v>318</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="108">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="108">
       <c r="A108" s="0" t="s">
         <v>319</v>
       </c>
@@ -6347,7 +6343,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="109">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="109">
       <c r="A109" s="0" t="s">
         <v>322</v>
       </c>
@@ -6367,7 +6363,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="110">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="110">
       <c r="A110" s="0" t="s">
         <v>324</v>
       </c>
@@ -6387,7 +6383,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="111">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="111">
       <c r="A111" s="0" t="s">
         <v>326</v>
       </c>
@@ -6410,7 +6406,7 @@
         <v>328</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="112">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="112">
       <c r="A112" s="0" t="s">
         <v>329</v>
       </c>
@@ -6433,7 +6429,7 @@
         <v>328</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="113">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="113">
       <c r="A113" s="0" t="s">
         <v>331</v>
       </c>
@@ -6456,7 +6452,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="114">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="114">
       <c r="A114" s="0" t="s">
         <v>334</v>
       </c>
@@ -6476,7 +6472,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="115">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="115">
       <c r="A115" s="0" t="s">
         <v>336</v>
       </c>
@@ -6502,7 +6498,7 @@
         <v>339</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="116">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="116">
       <c r="A116" s="0" t="s">
         <v>340</v>
       </c>
@@ -6531,7 +6527,7 @@
         <v>344</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="117">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="117">
       <c r="A117" s="0" t="s">
         <v>345</v>
       </c>
@@ -6551,7 +6547,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="118">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="118">
       <c r="A118" s="0" t="s">
         <v>348</v>
       </c>
@@ -6577,7 +6573,7 @@
         <v>351</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="119">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="119">
       <c r="A119" s="0" t="s">
         <v>352</v>
       </c>
@@ -6597,7 +6593,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="120">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="120">
       <c r="A120" s="0" t="s">
         <v>354</v>
       </c>
@@ -6617,7 +6613,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="121">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="121">
       <c r="A121" s="0" t="s">
         <v>356</v>
       </c>
@@ -6637,7 +6633,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="122">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="122">
       <c r="A122" s="0" t="s">
         <v>358</v>
       </c>
@@ -6660,7 +6656,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="123">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="123">
       <c r="A123" s="0" t="s">
         <v>361</v>
       </c>
@@ -6680,7 +6676,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="124">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="124">
       <c r="A124" s="0" t="s">
         <v>363</v>
       </c>
@@ -6703,7 +6699,7 @@
         <v>365</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="125">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="125">
       <c r="A125" s="0" t="s">
         <v>366</v>
       </c>
@@ -6726,7 +6722,7 @@
         <v>368</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="126">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="126">
       <c r="A126" s="0" t="s">
         <v>369</v>
       </c>
@@ -6749,7 +6745,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="127">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="127">
       <c r="A127" s="0" t="s">
         <v>372</v>
       </c>
@@ -6769,7 +6765,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="128">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="128">
       <c r="A128" s="0" t="s">
         <v>374</v>
       </c>
@@ -6792,7 +6788,7 @@
         <v>19</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="129">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="129">
       <c r="A129" s="0" t="s">
         <v>378</v>
       </c>
@@ -6815,7 +6811,7 @@
         <v>380</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="130">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="130">
       <c r="A130" s="0" t="s">
         <v>381</v>
       </c>
@@ -6838,7 +6834,7 @@
         <v>383</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="131">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="131">
       <c r="A131" s="0" t="s">
         <v>384</v>
       </c>
@@ -6858,7 +6854,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="132">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="132">
       <c r="A132" s="0" t="s">
         <v>387</v>
       </c>
@@ -6881,7 +6877,7 @@
         <v>389</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="133">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="133">
       <c r="A133" s="0" t="s">
         <v>390</v>
       </c>
@@ -6901,7 +6897,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="134">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="134">
       <c r="A134" s="0" t="s">
         <v>392</v>
       </c>
@@ -6921,7 +6917,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="135">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.05" outlineLevel="0" r="135">
       <c r="A135" s="0" t="s">
         <v>394</v>
       </c>
@@ -6941,7 +6937,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="136">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="136">
       <c r="A136" s="0" t="s">
         <v>396</v>
       </c>
@@ -6964,7 +6960,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="137">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="137">
       <c r="A137" s="0" t="s">
         <v>399</v>
       </c>
@@ -6984,7 +6980,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="138">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="138">
       <c r="A138" s="0" t="s">
         <v>401</v>
       </c>
@@ -7004,7 +7000,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="139">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="139">
       <c r="A139" s="0" t="s">
         <v>403</v>
       </c>
@@ -7030,7 +7026,7 @@
         <v>328</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="140">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="140">
       <c r="A140" s="0" t="s">
         <v>406</v>
       </c>
@@ -7056,7 +7052,7 @@
         <v>33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="141">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="141">
       <c r="A141" s="0" t="s">
         <v>409</v>
       </c>
@@ -7076,7 +7072,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="142">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="142">
       <c r="A142" s="0" t="s">
         <v>411</v>
       </c>
@@ -7102,7 +7098,7 @@
         <v>33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="143">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="143">
       <c r="A143" s="0" t="s">
         <v>414</v>
       </c>
@@ -7125,7 +7121,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="144">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="144">
       <c r="A144" s="0" t="s">
         <v>417</v>
       </c>
@@ -7154,7 +7150,7 @@
         <v>33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="145">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="145">
       <c r="A145" s="0" t="s">
         <v>421</v>
       </c>
@@ -7177,7 +7173,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="146">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="146">
       <c r="A146" s="0" t="s">
         <v>425</v>
       </c>
@@ -7200,7 +7196,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="147">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="147">
       <c r="A147" s="0" t="s">
         <v>428</v>
       </c>
@@ -7220,7 +7216,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="148">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="148">
       <c r="A148" s="0" t="s">
         <v>430</v>
       </c>
@@ -7240,7 +7236,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="149">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="149">
       <c r="A149" s="0" t="s">
         <v>432</v>
       </c>
@@ -7263,7 +7259,7 @@
         <v>434</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="150">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="150">
       <c r="A150" s="0" t="s">
         <v>435</v>
       </c>
@@ -7286,7 +7282,7 @@
         <v>434</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="151">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="151">
       <c r="A151" s="0" t="s">
         <v>437</v>
       </c>
@@ -7309,7 +7305,7 @@
         <v>33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="152">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="152">
       <c r="A152" s="0" t="s">
         <v>439</v>
       </c>
@@ -7332,7 +7328,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="153">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="153">
       <c r="A153" s="0" t="s">
         <v>442</v>
       </c>
@@ -7352,7 +7348,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="154">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="154">
       <c r="A154" s="0" t="s">
         <v>444</v>
       </c>
@@ -7375,7 +7371,7 @@
         <v>446</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="155">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="155">
       <c r="A155" s="0" t="s">
         <v>447</v>
       </c>
@@ -7395,7 +7391,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="156">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="156">
       <c r="A156" s="0" t="s">
         <v>449</v>
       </c>
@@ -7418,7 +7414,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="157">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="157">
       <c r="A157" s="0" t="s">
         <v>452</v>
       </c>
@@ -7444,7 +7440,7 @@
         <v>455</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="158">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="158">
       <c r="A158" s="0" t="s">
         <v>456</v>
       </c>
@@ -7467,7 +7463,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="159">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="159">
       <c r="A159" s="0" t="s">
         <v>459</v>
       </c>
@@ -7487,7 +7483,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="160">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="160">
       <c r="A160" s="0" t="s">
         <v>461</v>
       </c>
@@ -7507,7 +7503,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="161">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="161">
       <c r="A161" s="0" t="s">
         <v>463</v>
       </c>
@@ -7527,7 +7523,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="162">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="162">
       <c r="A162" s="0" t="s">
         <v>465</v>
       </c>
@@ -7547,7 +7543,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="163">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="163">
       <c r="A163" s="0" t="s">
         <v>467</v>
       </c>
@@ -7567,7 +7563,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="164">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="164">
       <c r="A164" s="0" t="s">
         <v>469</v>
       </c>
@@ -7590,7 +7586,7 @@
         <v>471</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="165">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="165">
       <c r="A165" s="0" t="s">
         <v>472</v>
       </c>
@@ -7613,7 +7609,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="166">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="166">
       <c r="A166" s="0" t="s">
         <v>475</v>
       </c>
@@ -7636,7 +7632,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="167">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="167">
       <c r="A167" s="0" t="s">
         <v>478</v>
       </c>
@@ -7659,7 +7655,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="168">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="168">
       <c r="A168" s="0" t="s">
         <v>481</v>
       </c>
@@ -7682,7 +7678,7 @@
         <v>483</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="169">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="169">
       <c r="A169" s="0" t="s">
         <v>484</v>
       </c>
@@ -7705,7 +7701,7 @@
         <v>486</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="170">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="170">
       <c r="A170" s="0" t="s">
         <v>487</v>
       </c>
@@ -7731,7 +7727,7 @@
         <v>33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="171">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="171">
       <c r="A171" s="0" t="s">
         <v>490</v>
       </c>
@@ -7757,7 +7753,7 @@
         <v>493</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="172">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="172">
       <c r="A172" s="0" t="s">
         <v>494</v>
       </c>
@@ -7780,7 +7776,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="173">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="173">
       <c r="A173" s="0" t="s">
         <v>497</v>
       </c>
@@ -7803,7 +7799,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="174">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="174">
       <c r="A174" s="0" t="s">
         <v>500</v>
       </c>
@@ -7823,7 +7819,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="175">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="175">
       <c r="A175" s="0" t="s">
         <v>503</v>
       </c>
@@ -7846,7 +7842,7 @@
         <v>505</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="176">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="176">
       <c r="A176" s="0" t="s">
         <v>506</v>
       </c>
@@ -7869,7 +7865,7 @@
         <v>508</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="177">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="177">
       <c r="A177" s="0" t="s">
         <v>509</v>
       </c>
@@ -7889,7 +7885,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="178">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="178">
       <c r="A178" s="0" t="s">
         <v>511</v>
       </c>
@@ -7912,7 +7908,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="179">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="179">
       <c r="A179" s="0" t="s">
         <v>514</v>
       </c>
@@ -7923,7 +7919,7 @@
         <v>516</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="180">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="180">
       <c r="A180" s="0" t="s">
         <v>517</v>
       </c>
@@ -7946,7 +7942,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="181">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="181">
       <c r="A181" s="0" t="s">
         <v>520</v>
       </c>
@@ -7969,7 +7965,7 @@
         <v>522</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="182">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="182">
       <c r="A182" s="0" t="s">
         <v>523</v>
       </c>
@@ -7989,7 +7985,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="183">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="183">
       <c r="A183" s="0" t="s">
         <v>526</v>
       </c>
@@ -8012,7 +8008,7 @@
         <v>528</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="184">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="184">
       <c r="A184" s="0" t="s">
         <v>529</v>
       </c>
@@ -8032,7 +8028,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="185">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="185">
       <c r="A185" s="0" t="s">
         <v>532</v>
       </c>
@@ -8052,7 +8048,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="186">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="186">
       <c r="A186" s="0" t="s">
         <v>534</v>
       </c>
@@ -8075,7 +8071,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="187">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="187">
       <c r="A187" s="0" t="s">
         <v>537</v>
       </c>
@@ -8095,7 +8091,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="188">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="188">
       <c r="A188" s="0" t="s">
         <v>539</v>
       </c>
@@ -8118,7 +8114,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="189">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="189">
       <c r="A189" s="0" t="s">
         <v>542</v>
       </c>
@@ -8141,7 +8137,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="190">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="190">
       <c r="A190" s="0" t="s">
         <v>545</v>
       </c>
@@ -8161,7 +8157,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="191">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="191">
       <c r="A191" s="0" t="s">
         <v>548</v>
       </c>
@@ -8181,7 +8177,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="192">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="192">
       <c r="A192" s="0" t="s">
         <v>551</v>
       </c>
@@ -8204,7 +8200,7 @@
         <v>554</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="193">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="193">
       <c r="A193" s="0" t="s">
         <v>555</v>
       </c>
@@ -8227,7 +8223,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="194">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="194">
       <c r="A194" s="0" t="s">
         <v>558</v>
       </c>
@@ -8250,7 +8246,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="195">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="195">
       <c r="A195" s="0" t="s">
         <v>561</v>
       </c>
@@ -8273,7 +8269,7 @@
         <v>563</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="196">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="196">
       <c r="A196" s="0" t="s">
         <v>561</v>
       </c>
@@ -8296,7 +8292,7 @@
         <v>563</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="197">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="197">
       <c r="A197" s="0" t="s">
         <v>565</v>
       </c>
@@ -8319,7 +8315,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="198">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="198">
       <c r="A198" s="0" t="s">
         <v>568</v>
       </c>
@@ -8345,7 +8341,7 @@
         <v>571</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="199">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="199">
       <c r="A199" s="0" t="s">
         <v>572</v>
       </c>
@@ -8365,7 +8361,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="200">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="200">
       <c r="A200" s="0" t="s">
         <v>574</v>
       </c>
@@ -8391,7 +8387,7 @@
         <v>577</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="201">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="201">
       <c r="A201" s="0" t="s">
         <v>578</v>
       </c>
@@ -8417,7 +8413,7 @@
         <v>581</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="202">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="202">
       <c r="A202" s="0" t="s">
         <v>582</v>
       </c>
@@ -8437,7 +8433,7 @@
         <v>19</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="203">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="203">
       <c r="A203" s="0" t="s">
         <v>584</v>
       </c>
@@ -8457,7 +8453,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="204">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="204">
       <c r="A204" s="0" t="s">
         <v>586</v>
       </c>
@@ -8480,7 +8476,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="205">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="205">
       <c r="A205" s="0" t="s">
         <v>589</v>
       </c>
@@ -8503,7 +8499,7 @@
         <v>591</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="206">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="206">
       <c r="A206" s="0" t="s">
         <v>592</v>
       </c>
@@ -8526,7 +8522,7 @@
         <v>19</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="207">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="207">
       <c r="A207" s="0" t="s">
         <v>595</v>
       </c>
@@ -8549,7 +8545,7 @@
         <v>597</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="208">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="208">
       <c r="A208" s="0" t="s">
         <v>598</v>
       </c>
@@ -8572,7 +8568,7 @@
         <v>600</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="209">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="209">
       <c r="A209" s="0" t="s">
         <v>601</v>
       </c>
@@ -8592,7 +8588,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="210">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="210">
       <c r="A210" s="0" t="s">
         <v>603</v>
       </c>
@@ -8615,7 +8611,7 @@
         <v>605</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="211">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="211">
       <c r="A211" s="0" t="s">
         <v>606</v>
       </c>
@@ -8635,7 +8631,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="212">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="212">
       <c r="A212" s="0" t="s">
         <v>608</v>
       </c>
@@ -8655,7 +8651,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="213">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="213">
       <c r="A213" s="0" t="s">
         <v>610</v>
       </c>
@@ -8675,7 +8671,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="214">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="214">
       <c r="A214" s="0" t="s">
         <v>612</v>
       </c>
@@ -8695,7 +8691,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="215">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="215">
       <c r="A215" s="0" t="s">
         <v>614</v>
       </c>
@@ -8715,7 +8711,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="216">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="216">
       <c r="A216" s="0" t="s">
         <v>616</v>
       </c>
@@ -8735,7 +8731,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="217">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="217">
       <c r="A217" s="0" t="s">
         <v>618</v>
       </c>
@@ -8755,7 +8751,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="218">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="218">
       <c r="A218" s="0" t="s">
         <v>620</v>
       </c>
@@ -8778,7 +8774,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="219">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="219">
       <c r="A219" s="0" t="s">
         <v>623</v>
       </c>
@@ -8804,7 +8800,7 @@
         <v>626</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="220">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="220">
       <c r="A220" s="0" t="s">
         <v>627</v>
       </c>
@@ -8830,7 +8826,7 @@
         <v>630</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="221">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="221">
       <c r="A221" s="0" t="s">
         <v>631</v>
       </c>
@@ -8856,7 +8852,7 @@
         <v>630</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="222">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="222">
       <c r="A222" s="0" t="s">
         <v>634</v>
       </c>
@@ -8882,7 +8878,7 @@
         <v>630</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="223">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="223">
       <c r="A223" s="0" t="s">
         <v>637</v>
       </c>
@@ -8908,7 +8904,7 @@
         <v>640</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="224">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="224">
       <c r="A224" s="0" t="s">
         <v>641</v>
       </c>
@@ -8931,7 +8927,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="225">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="225">
       <c r="A225" s="0" t="s">
         <v>644</v>
       </c>
@@ -8957,7 +8953,7 @@
         <v>647</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="226">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="226">
       <c r="A226" s="0" t="s">
         <v>648</v>
       </c>
@@ -8980,7 +8976,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="227">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="227">
       <c r="A227" s="0" t="s">
         <v>651</v>
       </c>
@@ -9000,7 +8996,7 @@
         <v>653</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="228">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="228">
       <c r="A228" s="0" t="s">
         <v>654</v>
       </c>
@@ -9023,7 +9019,7 @@
         <v>656</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="229">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="229">
       <c r="A229" s="0" t="s">
         <v>657</v>
       </c>
@@ -9046,7 +9042,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="230">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="230">
       <c r="A230" s="0" t="s">
         <v>660</v>
       </c>
@@ -9069,7 +9065,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="231">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="231">
       <c r="A231" s="0" t="s">
         <v>663</v>
       </c>
@@ -9092,7 +9088,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="232">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="232">
       <c r="A232" s="0" t="s">
         <v>666</v>
       </c>
@@ -9112,7 +9108,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="233">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="233">
       <c r="A233" s="0" t="s">
         <v>668</v>
       </c>
@@ -9135,7 +9131,7 @@
         <v>670</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="234">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="234">
       <c r="A234" s="0" t="s">
         <v>671</v>
       </c>
@@ -9161,7 +9157,7 @@
         <v>675</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="235">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="235">
       <c r="A235" s="0" t="s">
         <v>676</v>
       </c>
@@ -9184,7 +9180,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="236">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="236">
       <c r="A236" s="0" t="s">
         <v>679</v>
       </c>
@@ -9204,7 +9200,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="237">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="237">
       <c r="A237" s="0" t="s">
         <v>681</v>
       </c>
@@ -9224,7 +9220,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="238">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="238">
       <c r="A238" s="0" t="s">
         <v>683</v>
       </c>
@@ -9244,7 +9240,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="239">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="239">
       <c r="A239" s="0" t="s">
         <v>685</v>
       </c>
@@ -9264,7 +9260,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="240">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="240">
       <c r="A240" s="0" t="s">
         <v>687</v>
       </c>
@@ -9284,7 +9280,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="241">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="241">
       <c r="A241" s="0" t="s">
         <v>689</v>
       </c>
@@ -9304,7 +9300,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="242">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="242">
       <c r="A242" s="0" t="s">
         <v>691</v>
       </c>
@@ -9327,7 +9323,7 @@
         <v>693</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="243">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="243">
       <c r="A243" s="0" t="s">
         <v>694</v>
       </c>
@@ -9350,7 +9346,7 @@
         <v>696</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="244">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="244">
       <c r="A244" s="0" t="s">
         <v>697</v>
       </c>
@@ -9376,7 +9372,7 @@
         <v>700</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="245">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="245">
       <c r="A245" s="0" t="s">
         <v>701</v>
       </c>
@@ -9396,7 +9392,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="246">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="246">
       <c r="A246" s="0" t="s">
         <v>703</v>
       </c>
@@ -9419,7 +9415,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="247">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="247">
       <c r="A247" s="0" t="s">
         <v>706</v>
       </c>
@@ -9445,7 +9441,7 @@
         <v>630</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="248">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="248">
       <c r="A248" s="0" t="s">
         <v>710</v>
       </c>
@@ -9468,7 +9464,7 @@
         <v>712</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="249">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="249">
       <c r="A249" s="0" t="s">
         <v>713</v>
       </c>
@@ -9491,7 +9487,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="250">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="250">
       <c r="A250" s="0" t="s">
         <v>716</v>
       </c>
@@ -9514,7 +9510,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="251">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="251">
       <c r="A251" s="0" t="s">
         <v>719</v>
       </c>
@@ -9537,7 +9533,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="252">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="252">
       <c r="A252" s="0" t="s">
         <v>721</v>
       </c>
@@ -9560,7 +9556,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="253">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="253">
       <c r="A253" s="0" t="s">
         <v>722</v>
       </c>
@@ -9583,7 +9579,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="254">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="254">
       <c r="A254" s="0" t="s">
         <v>725</v>
       </c>
@@ -9606,7 +9602,7 @@
         <v>727</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="255">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="255">
       <c r="A255" s="0" t="s">
         <v>728</v>
       </c>
@@ -9626,7 +9622,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="256">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="256">
       <c r="A256" s="0" t="s">
         <v>730</v>
       </c>
@@ -9652,7 +9648,7 @@
         <v>734</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="257">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="257">
       <c r="A257" s="0" t="s">
         <v>735</v>
       </c>
@@ -9675,7 +9671,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="258">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="258">
       <c r="A258" s="0" t="s">
         <v>738</v>
       </c>
@@ -9701,7 +9697,7 @@
         <v>741</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="259">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="259">
       <c r="A259" s="0" t="s">
         <v>742</v>
       </c>
@@ -9721,7 +9717,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="260">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="260">
       <c r="A260" s="0" t="s">
         <v>744</v>
       </c>
@@ -9744,7 +9740,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="261">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="261">
       <c r="A261" s="0" t="s">
         <v>747</v>
       </c>
@@ -9770,7 +9766,7 @@
         <v>750</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="262">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="262">
       <c r="A262" s="0" t="s">
         <v>751</v>
       </c>
@@ -9796,7 +9792,7 @@
         <v>755</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="263">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="263">
       <c r="A263" s="0" t="s">
         <v>756</v>
       </c>
@@ -9822,7 +9818,7 @@
         <v>759</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="264">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="264">
       <c r="A264" s="0" t="s">
         <v>760</v>
       </c>
@@ -9842,7 +9838,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="265">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="265">
       <c r="A265" s="0" t="s">
         <v>762</v>
       </c>
@@ -9868,7 +9864,7 @@
         <v>765</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="266">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="266">
       <c r="A266" s="0" t="s">
         <v>766</v>
       </c>
@@ -9891,7 +9887,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="267">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="267">
       <c r="A267" s="0" t="s">
         <v>770</v>
       </c>
@@ -9917,7 +9913,7 @@
         <v>773</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="268">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="268">
       <c r="A268" s="0" t="s">
         <v>774</v>
       </c>
@@ -9940,7 +9936,7 @@
         <v>776</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="269">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="269">
       <c r="A269" s="0" t="s">
         <v>777</v>
       </c>
@@ -9951,7 +9947,7 @@
         <v>15</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="270">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="270">
       <c r="A270" s="0" t="s">
         <v>779</v>
       </c>
@@ -9971,7 +9967,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="271">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="271">
       <c r="A271" s="0" t="s">
         <v>781</v>
       </c>
@@ -9991,7 +9987,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="272">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="272">
       <c r="A272" s="0" t="s">
         <v>782</v>
       </c>
@@ -10017,7 +10013,7 @@
         <v>785</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="273">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="273">
       <c r="A273" s="0" t="s">
         <v>786</v>
       </c>
@@ -10046,7 +10042,7 @@
         <v>789</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="274">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="274">
       <c r="A274" s="0" t="s">
         <v>790</v>
       </c>
@@ -10069,7 +10065,7 @@
         <v>785</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="275">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="275">
       <c r="A275" s="0" t="s">
         <v>792</v>
       </c>
@@ -10089,7 +10085,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="276">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="276">
       <c r="A276" s="0" t="s">
         <v>794</v>
       </c>
@@ -10112,7 +10108,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="277">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="277">
       <c r="A277" s="0" t="s">
         <v>797</v>
       </c>
@@ -10132,7 +10128,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="278">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="278">
       <c r="A278" s="0" t="s">
         <v>799</v>
       </c>
@@ -10152,7 +10148,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="279">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="279">
       <c r="A279" s="0" t="s">
         <v>801</v>
       </c>
@@ -10172,7 +10168,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="280">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="280">
       <c r="A280" s="0" t="s">
         <v>803</v>
       </c>
@@ -10198,7 +10194,7 @@
         <v>806</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="281">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="281">
       <c r="A281" s="0" t="s">
         <v>807</v>
       </c>
@@ -10221,7 +10217,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="282">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="282">
       <c r="A282" s="0" t="s">
         <v>809</v>
       </c>
@@ -10244,7 +10240,7 @@
         <v>810</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="283">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="283">
       <c r="A283" s="0" t="s">
         <v>811</v>
       </c>
@@ -10267,7 +10263,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="284">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="284">
       <c r="A284" s="0" t="s">
         <v>814</v>
       </c>
@@ -10290,7 +10286,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="285">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="285">
       <c r="A285" s="0" t="s">
         <v>817</v>
       </c>
@@ -10313,7 +10309,7 @@
         <v>819</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="286">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="286">
       <c r="A286" s="0" t="s">
         <v>820</v>
       </c>
@@ -10333,7 +10329,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="287">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="287">
       <c r="A287" s="0" t="s">
         <v>823</v>
       </c>
@@ -10353,7 +10349,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="288">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="288">
       <c r="A288" s="0" t="s">
         <v>825</v>
       </c>
@@ -10376,7 +10372,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="289">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="289">
       <c r="A289" s="0" t="s">
         <v>828</v>
       </c>
@@ -10399,7 +10395,7 @@
         <v>830</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="290">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="290">
       <c r="A290" s="0" t="s">
         <v>831</v>
       </c>
@@ -10422,7 +10418,7 @@
         <v>833</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="291">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="291">
       <c r="A291" s="0" t="s">
         <v>834</v>
       </c>
@@ -10442,7 +10438,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="292">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="292">
       <c r="A292" s="0" t="s">
         <v>836</v>
       </c>
@@ -10465,7 +10461,7 @@
         <v>838</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="293">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="293">
       <c r="A293" s="0" t="s">
         <v>839</v>
       </c>
@@ -10488,7 +10484,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="294">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="294">
       <c r="A294" s="0" t="s">
         <v>842</v>
       </c>
@@ -10511,7 +10507,7 @@
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="295">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="295">
       <c r="A295" s="0" t="s">
         <v>843</v>
       </c>
@@ -10531,7 +10527,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="296">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="296">
       <c r="A296" s="0" t="s">
         <v>845</v>
       </c>
@@ -10557,7 +10553,7 @@
         <v>848</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="297">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="297">
       <c r="A297" s="0" t="s">
         <v>849</v>
       </c>
@@ -10583,7 +10579,7 @@
         <v>852</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="298">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="298">
       <c r="A298" s="0" t="s">
         <v>853</v>
       </c>
@@ -10609,7 +10605,7 @@
         <v>852</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="299">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="299">
       <c r="A299" s="0" t="s">
         <v>854</v>
       </c>
@@ -10635,7 +10631,7 @@
         <v>857</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="300">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="300">
       <c r="A300" s="0" t="s">
         <v>858</v>
       </c>
@@ -10658,7 +10654,7 @@
         <v>860</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="301">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="301">
       <c r="A301" s="0" t="s">
         <v>861</v>
       </c>
@@ -10681,7 +10677,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="302">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="302">
       <c r="A302" s="0" t="s">
         <v>864</v>
       </c>
@@ -10704,7 +10700,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="303">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="303">
       <c r="A303" s="0" t="s">
         <v>867</v>
       </c>
@@ -10727,7 +10723,7 @@
         <v>869</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="304">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="304">
       <c r="A304" s="0" t="s">
         <v>870</v>
       </c>
@@ -10747,7 +10743,7 @@
         <v>872</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="305">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="305">
       <c r="A305" s="0" t="s">
         <v>873</v>
       </c>
@@ -10770,7 +10766,7 @@
         <v>875</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="306">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="306">
       <c r="A306" s="0" t="s">
         <v>876</v>
       </c>
@@ -10793,7 +10789,7 @@
         <v>878</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="307">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="307">
       <c r="A307" s="0" t="s">
         <v>879</v>
       </c>
@@ -10819,7 +10815,7 @@
         <v>883</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="308">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="308">
       <c r="A308" s="0" t="s">
         <v>884</v>
       </c>
@@ -10845,7 +10841,7 @@
         <v>887</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="309">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="309">
       <c r="A309" s="0" t="s">
         <v>888</v>
       </c>
@@ -10868,7 +10864,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="310">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="310">
       <c r="A310" s="0" t="s">
         <v>891</v>
       </c>
@@ -10888,7 +10884,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="311">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="311">
       <c r="A311" s="0" t="s">
         <v>893</v>
       </c>
@@ -10911,7 +10907,7 @@
         <v>895</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="312">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="312">
       <c r="A312" s="0" t="s">
         <v>896</v>
       </c>
@@ -10934,7 +10930,7 @@
         <v>895</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="313">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="313">
       <c r="A313" s="0" t="s">
         <v>899</v>
       </c>
@@ -10957,7 +10953,7 @@
         <v>33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="314">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="314">
       <c r="A314" s="0" t="s">
         <v>901</v>
       </c>
@@ -10977,7 +10973,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="315">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="315">
       <c r="A315" s="0" t="s">
         <v>903</v>
       </c>
@@ -11003,7 +10999,7 @@
         <v>906</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="316">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="316">
       <c r="A316" s="0" t="s">
         <v>907</v>
       </c>
@@ -11026,7 +11022,7 @@
         <v>33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="317">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="317">
       <c r="A317" s="0" t="s">
         <v>909</v>
       </c>
@@ -11052,7 +11048,7 @@
         <v>912</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="318">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="318">
       <c r="A318" s="0" t="s">
         <v>913</v>
       </c>
@@ -11078,7 +11074,7 @@
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="319">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="319">
       <c r="A319" s="0" t="s">
         <v>916</v>
       </c>
@@ -11098,7 +11094,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="320">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="320">
       <c r="A320" s="0" t="s">
         <v>918</v>
       </c>
@@ -11124,7 +11120,7 @@
         <v>921</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="321">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="321">
       <c r="A321" s="0" t="s">
         <v>922</v>
       </c>
@@ -11150,7 +11146,7 @@
         <v>925</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="322">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="322">
       <c r="A322" s="0" t="s">
         <v>926</v>
       </c>
@@ -11173,7 +11169,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="323">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="323">
       <c r="A323" s="0" t="s">
         <v>929</v>
       </c>
@@ -11196,7 +11192,7 @@
         <v>931</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="324">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="324">
       <c r="A324" s="0" t="s">
         <v>932</v>
       </c>
@@ -11219,7 +11215,7 @@
         <v>934</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="325">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="325">
       <c r="A325" s="0" t="s">
         <v>935</v>
       </c>
@@ -11239,7 +11235,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="326">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="326">
       <c r="A326" s="0" t="s">
         <v>937</v>
       </c>
@@ -11259,7 +11255,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="327">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="327">
       <c r="A327" s="0" t="s">
         <v>939</v>
       </c>
@@ -11282,7 +11278,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="328">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="328">
       <c r="A328" s="0" t="s">
         <v>942</v>
       </c>
@@ -11302,7 +11298,7 @@
         <v>944</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="329">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="329">
       <c r="A329" s="0" t="s">
         <v>945</v>
       </c>
@@ -11325,7 +11321,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="330">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="330">
       <c r="A330" s="0" t="s">
         <v>948</v>
       </c>
@@ -11345,7 +11341,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="331">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="331">
       <c r="A331" s="0" t="s">
         <v>950</v>
       </c>
@@ -11365,7 +11361,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="332">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="332">
       <c r="A332" s="0" t="s">
         <v>952</v>
       </c>
@@ -11385,7 +11381,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="333">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="333">
       <c r="A333" s="0" t="s">
         <v>954</v>
       </c>
@@ -11405,7 +11401,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="334">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="334">
       <c r="A334" s="0" t="s">
         <v>956</v>
       </c>
@@ -11428,7 +11424,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="335">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="335">
       <c r="A335" s="0" t="s">
         <v>959</v>
       </c>
@@ -11451,7 +11447,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="336">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="336">
       <c r="A336" s="0" t="s">
         <v>962</v>
       </c>
@@ -11471,7 +11467,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="337">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="337">
       <c r="A337" s="0" t="s">
         <v>964</v>
       </c>
@@ -11494,7 +11490,7 @@
         <v>19</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="338">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="338">
       <c r="A338" s="0" t="s">
         <v>967</v>
       </c>
@@ -11514,7 +11510,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="339">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="339">
       <c r="A339" s="0" t="s">
         <v>969</v>
       </c>
@@ -11537,7 +11533,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="340">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="340">
       <c r="A340" s="0" t="s">
         <v>972</v>
       </c>
@@ -11560,7 +11556,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="341">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="341">
       <c r="A341" s="0" t="s">
         <v>975</v>
       </c>
@@ -11583,7 +11579,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="342">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="342">
       <c r="A342" s="0" t="s">
         <v>978</v>
       </c>
@@ -11603,7 +11599,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="343">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="343">
       <c r="A343" s="0" t="s">
         <v>980</v>
       </c>
@@ -11629,7 +11625,7 @@
         <v>983</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="344">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="344">
       <c r="A344" s="0" t="s">
         <v>984</v>
       </c>
@@ -11652,7 +11648,7 @@
         <v>986</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="345">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="345">
       <c r="A345" s="0" t="s">
         <v>987</v>
       </c>
@@ -11675,7 +11671,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="346">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="346">
       <c r="A346" s="0" t="s">
         <v>990</v>
       </c>
@@ -11695,7 +11691,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="347">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="347">
       <c r="A347" s="0" t="s">
         <v>992</v>
       </c>
@@ -11718,7 +11714,7 @@
         <v>994</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="348">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="348">
       <c r="A348" s="0" t="s">
         <v>995</v>
       </c>
@@ -11741,7 +11737,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="349">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="349">
       <c r="A349" s="0" t="s">
         <v>998</v>
       </c>
@@ -11764,7 +11760,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="350">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="350">
       <c r="A350" s="0" t="s">
         <v>998</v>
       </c>
@@ -11787,7 +11783,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="351">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="351">
       <c r="A351" s="0" t="s">
         <v>1001</v>
       </c>
@@ -11810,7 +11806,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="352">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="352">
       <c r="A352" s="0" t="s">
         <v>1004</v>
       </c>
@@ -11830,7 +11826,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="353">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="353">
       <c r="A353" s="0" t="s">
         <v>1006</v>
       </c>
@@ -11856,7 +11852,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="354">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="354">
       <c r="A354" s="0" t="s">
         <v>1010</v>
       </c>
@@ -11876,7 +11872,7 @@
         <v>19</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="355">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="355">
       <c r="A355" s="0" t="s">
         <v>1012</v>
       </c>
@@ -11899,7 +11895,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="356">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="356">
       <c r="A356" s="0" t="s">
         <v>1015</v>
       </c>
@@ -11919,7 +11915,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="357">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="357">
       <c r="A357" s="0" t="s">
         <v>1017</v>
       </c>
@@ -11939,7 +11935,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="358">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="358">
       <c r="A358" s="0" t="s">
         <v>1019</v>
       </c>
@@ -11959,7 +11955,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="359">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="359">
       <c r="A359" s="0" t="s">
         <v>1021</v>
       </c>
@@ -11979,7 +11975,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="360">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="360">
       <c r="A360" s="0" t="s">
         <v>1023</v>
       </c>
@@ -12005,7 +12001,7 @@
         <v>208</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="361">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="361">
       <c r="A361" s="0" t="s">
         <v>1026</v>
       </c>
@@ -12028,7 +12024,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="362">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="362">
       <c r="A362" s="0" t="s">
         <v>1029</v>
       </c>
@@ -12048,7 +12044,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="363">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="363">
       <c r="A363" s="0" t="s">
         <v>1031</v>
       </c>
@@ -12071,7 +12067,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="364">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="364">
       <c r="A364" s="0" t="s">
         <v>1034</v>
       </c>
@@ -12097,7 +12093,7 @@
         <v>33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="365">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="365">
       <c r="A365" s="0" t="s">
         <v>1037</v>
       </c>
@@ -12120,7 +12116,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="366">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="366">
       <c r="A366" s="0" t="s">
         <v>1040</v>
       </c>
@@ -12140,7 +12136,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="367">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="367">
       <c r="A367" s="0" t="s">
         <v>1042</v>
       </c>
@@ -12160,7 +12156,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="368">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="368">
       <c r="A368" s="0" t="s">
         <v>1044</v>
       </c>
@@ -12180,7 +12176,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="369">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="369">
       <c r="A369" s="0" t="s">
         <v>1046</v>
       </c>
@@ -12203,7 +12199,7 @@
         <v>1048</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="370">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="370">
       <c r="A370" s="0" t="s">
         <v>1049</v>
       </c>
@@ -12226,7 +12222,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="371">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="371">
       <c r="A371" s="0" t="s">
         <v>1052</v>
       </c>
@@ -12252,7 +12248,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="372">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="372">
       <c r="A372" s="0" t="s">
         <v>1056</v>
       </c>
@@ -12279,7 +12275,7 @@
       </c>
       <c r="I372" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="373">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="373">
       <c r="A373" s="0" t="s">
         <v>1057</v>
       </c>
@@ -12305,7 +12301,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="374">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="374">
       <c r="A374" s="0" t="s">
         <v>1058</v>
       </c>
@@ -12331,7 +12327,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="375">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="375">
       <c r="A375" s="0" t="s">
         <v>1059</v>
       </c>
@@ -12357,7 +12353,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="376">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="376">
       <c r="A376" s="0" t="s">
         <v>1060</v>
       </c>
@@ -12383,7 +12379,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="377">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="377">
       <c r="A377" s="0" t="s">
         <v>1061</v>
       </c>
@@ -12403,7 +12399,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="378">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="378">
       <c r="A378" s="0" t="s">
         <v>1063</v>
       </c>
@@ -12426,7 +12422,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="379">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="379">
       <c r="A379" s="0" t="s">
         <v>1066</v>
       </c>
@@ -12452,7 +12448,7 @@
         <v>1069</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="380">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="380">
       <c r="A380" s="0" t="s">
         <v>1070</v>
       </c>
@@ -12472,7 +12468,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="381">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="381">
       <c r="A381" s="0" t="s">
         <v>1072</v>
       </c>
@@ -12496,7 +12492,7 @@
       </c>
       <c r="I381" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="382">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="382">
       <c r="A382" s="0" t="s">
         <v>1075</v>
       </c>
@@ -12516,7 +12512,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="383">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="383">
       <c r="A383" s="0" t="s">
         <v>1077</v>
       </c>
@@ -12536,7 +12532,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="384">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="384">
       <c r="A384" s="0" t="s">
         <v>1079</v>
       </c>
@@ -12562,7 +12558,7 @@
         <v>33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="385">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="385">
       <c r="A385" s="0" t="s">
         <v>1082</v>
       </c>
@@ -12582,7 +12578,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="386">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="386">
       <c r="A386" s="0" t="s">
         <v>1084</v>
       </c>
@@ -12605,7 +12601,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="387">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="387">
       <c r="A387" s="0" t="s">
         <v>1087</v>
       </c>
@@ -12628,7 +12624,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="388">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="388">
       <c r="A388" s="0" t="s">
         <v>1090</v>
       </c>
@@ -12648,7 +12644,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="389">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="389">
       <c r="A389" s="0" t="s">
         <v>1092</v>
       </c>
@@ -12671,7 +12667,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="390">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="390">
       <c r="A390" s="0" t="s">
         <v>1095</v>
       </c>
@@ -12694,7 +12690,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="391">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="391">
       <c r="A391" s="0" t="s">
         <v>1098</v>
       </c>
@@ -12714,7 +12710,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="392">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="392">
       <c r="A392" s="0" t="s">
         <v>1100</v>
       </c>
@@ -12737,7 +12733,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="393">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="393">
       <c r="A393" s="0" t="s">
         <v>1103</v>
       </c>
@@ -12760,7 +12756,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="394">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="394">
       <c r="A394" s="0" t="s">
         <v>1106</v>
       </c>
@@ -12786,7 +12782,7 @@
         <v>1109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="395">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="395">
       <c r="A395" s="0" t="s">
         <v>1110</v>
       </c>
@@ -12809,7 +12805,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="396">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="396">
       <c r="A396" s="0" t="s">
         <v>1113</v>
       </c>
@@ -12829,7 +12825,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="397">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="397">
       <c r="A397" s="0" t="s">
         <v>1115</v>
       </c>
@@ -12852,7 +12848,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="398">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="398">
       <c r="A398" s="0" t="s">
         <v>1118</v>
       </c>
@@ -12875,7 +12871,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="399">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="399">
       <c r="A399" s="0" t="s">
         <v>1121</v>
       </c>
@@ -12895,7 +12891,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="400">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="400">
       <c r="A400" s="0" t="s">
         <v>1123</v>
       </c>
@@ -12919,7 +12915,7 @@
       </c>
       <c r="I400" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="401">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="401">
       <c r="A401" s="2" t="s">
         <v>1126</v>
       </c>
@@ -12940,7 +12936,7 @@
       </c>
       <c r="H401" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="402">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="402">
       <c r="A402" s="0" t="s">
         <v>1128</v>
       </c>
@@ -12960,7 +12956,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="403">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="403">
       <c r="A403" s="0" t="s">
         <v>1130</v>
       </c>
@@ -12980,7 +12976,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="404">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="404">
       <c r="A404" s="0" t="s">
         <v>1132</v>
       </c>
@@ -13000,7 +12996,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="405">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="405">
       <c r="A405" s="0" t="s">
         <v>1134</v>
       </c>
@@ -13020,7 +13016,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="406">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="406">
       <c r="A406" s="0" t="s">
         <v>1136</v>
       </c>
@@ -13043,7 +13039,7 @@
         <v>1138</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="407">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="407">
       <c r="A407" s="0" t="s">
         <v>1139</v>
       </c>
@@ -13063,7 +13059,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="408">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="408">
       <c r="A408" s="0" t="s">
         <v>1141</v>
       </c>
@@ -13086,7 +13082,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="409">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="409">
       <c r="A409" s="0" t="s">
         <v>1144</v>
       </c>
@@ -13106,7 +13102,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="410">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="410">
       <c r="A410" s="0" t="s">
         <v>1146</v>
       </c>
@@ -13126,7 +13122,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="411">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="411">
       <c r="A411" s="0" t="s">
         <v>1148</v>
       </c>
@@ -13149,7 +13145,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="412">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="412">
       <c r="A412" s="0" t="s">
         <v>1151</v>
       </c>
@@ -13169,7 +13165,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="413">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="413">
       <c r="A413" s="0" t="s">
         <v>1153</v>
       </c>
@@ -13192,7 +13188,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="414">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="414">
       <c r="A414" s="0" t="s">
         <v>1156</v>
       </c>
@@ -13215,7 +13211,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="415">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="415">
       <c r="A415" s="0" t="s">
         <v>1159</v>
       </c>
@@ -13235,7 +13231,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="416">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="416">
       <c r="A416" s="0" t="s">
         <v>1161</v>
       </c>
@@ -13255,7 +13251,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="417">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="417">
       <c r="A417" s="0" t="s">
         <v>1163</v>
       </c>
@@ -13278,7 +13274,7 @@
         <v>1165</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="418">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="418">
       <c r="A418" s="0" t="s">
         <v>1166</v>
       </c>
@@ -13301,7 +13297,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="419">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="419">
       <c r="A419" s="0" t="s">
         <v>1169</v>
       </c>
@@ -13321,7 +13317,7 @@
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="420">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="420">
       <c r="A420" s="0" t="s">
         <v>1171</v>
       </c>
@@ -13341,7 +13337,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="421">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="421">
       <c r="A421" s="0" t="s">
         <v>1173</v>
       </c>
@@ -13364,7 +13360,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="422">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="422">
       <c r="A422" s="0" t="s">
         <v>1176</v>
       </c>
@@ -13387,7 +13383,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="423">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="423">
       <c r="A423" s="0" t="s">
         <v>1179</v>
       </c>
@@ -13410,7 +13406,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="424">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="424">
       <c r="A424" s="0" t="s">
         <v>1182</v>
       </c>
@@ -13433,7 +13429,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="425">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="425">
       <c r="A425" s="0" t="s">
         <v>1185</v>
       </c>
@@ -13459,7 +13455,7 @@
         <v>208</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="426">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="426">
       <c r="A426" s="0" t="s">
         <v>1188</v>
       </c>
@@ -13479,7 +13475,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="427">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="427">
       <c r="A427" s="0" t="s">
         <v>1190</v>
       </c>
@@ -13499,7 +13495,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="428">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="428">
       <c r="A428" s="0" t="s">
         <v>1192</v>
       </c>
@@ -13522,7 +13518,7 @@
         <v>1194</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="429">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="429">
       <c r="A429" s="0" t="s">
         <v>1195</v>
       </c>
@@ -13545,7 +13541,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="430">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="430">
       <c r="A430" s="0" t="s">
         <v>1198</v>
       </c>
@@ -13568,7 +13564,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="431">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="431">
       <c r="A431" s="0" t="s">
         <v>1201</v>
       </c>
@@ -13591,7 +13587,7 @@
         <v>1203</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="432">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="432">
       <c r="A432" s="0" t="s">
         <v>1204</v>
       </c>
@@ -13614,7 +13610,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="433">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="433">
       <c r="A433" s="0" t="s">
         <v>1207</v>
       </c>
@@ -13634,7 +13630,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="434">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.05" outlineLevel="0" r="434">
       <c r="A434" s="0" t="s">
         <v>1209</v>
       </c>
@@ -13657,7 +13653,7 @@
         <v>1211</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="435">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="435">
       <c r="A435" s="0" t="s">
         <v>1212</v>
       </c>
@@ -13680,7 +13676,7 @@
         <v>1211</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="436">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="436">
       <c r="A436" s="0" t="s">
         <v>1214</v>
       </c>
@@ -13703,7 +13699,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="437">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="437">
       <c r="A437" s="0" t="s">
         <v>1217</v>
       </c>
@@ -13726,7 +13722,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="438">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="438">
       <c r="A438" s="0" t="s">
         <v>1220</v>
       </c>
@@ -13749,7 +13745,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="439">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="439">
       <c r="A439" s="0" t="s">
         <v>1223</v>
       </c>
@@ -13772,7 +13768,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="440">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="440">
       <c r="A440" s="0" t="s">
         <v>1226</v>
       </c>
@@ -13798,7 +13794,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="441">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="441">
       <c r="A441" s="0" t="s">
         <v>1229</v>
       </c>
@@ -13824,7 +13820,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="442">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="442">
       <c r="A442" s="0" t="s">
         <v>1232</v>
       </c>
@@ -13847,7 +13843,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="443">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="443">
       <c r="A443" s="0" t="s">
         <v>1235</v>
       </c>
@@ -13873,7 +13869,7 @@
         <v>1238</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="444">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="444">
       <c r="A444" s="0" t="s">
         <v>1239</v>
       </c>
@@ -13939,7 +13935,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="257" min="1" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="257" min="1" style="0" width="8.57647058823529"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -13964,7 +13960,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="257" min="1" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="257" min="1" style="0" width="8.57647058823529"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>